<commit_message>
Updated versions of diagrams and CI list
</commit_message>
<xml_diff>
--- a/Documents/Configuration Items List v1.0.xlsx
+++ b/Documents/Configuration Items List v1.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>Configuration Item Name</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Use cases</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>CI List v1.0</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +154,14 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -217,11 +231,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF404040"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -249,6 +272,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,56 +594,45 @@
     <col min="7" max="7" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+    <row r="3" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
-        <v>42141</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="6">
-        <v>42146</v>
+        <v>42141</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>6</v>
@@ -626,52 +641,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
       <c r="D4" s="6">
-        <v>42149</v>
+        <v>42146</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
       </c>
       <c r="D5" s="6">
-        <v>42155</v>
+        <v>42149</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -686,12 +701,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -706,35 +721,35 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
+        <v>42155</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="6">
-        <v>42148</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D9" s="6">
         <v>42148</v>
@@ -748,13 +763,13 @@
     </row>
     <row r="10" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="6">
         <v>42148</v>
@@ -768,30 +783,30 @@
     </row>
     <row r="11" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D11" s="6">
-        <v>42139</v>
+        <v>42148</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5">
         <v>3</v>
@@ -803,38 +818,38 @@
         <v>6</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="6">
-        <v>42157</v>
+        <v>42139</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
       </c>
       <c r="D14" s="6">
         <v>42157</v>
@@ -843,38 +858,38 @@
         <v>6</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="6">
+        <v>42157</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1</v>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>26</v>
@@ -883,10 +898,34 @@
         <v>6</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>